<commit_message>
Excel formatting - color coding and clickable links
</commit_message>
<xml_diff>
--- a/email_extractor/output/2026_01_13_PreMQL (2).xlsx
+++ b/email_extractor/output/2026_01_13_PreMQL (2).xlsx
@@ -3,13 +3,15 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Validation" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Review" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Validation'!$A$1:$BD$38</definedName>
+  </definedNames>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
@@ -98,8 +100,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFFE699"/>
-          <bgColor rgb="FFFFE699"/>
+          <fgColor rgb="FFF8CBAD"/>
+          <bgColor rgb="FFF8CBAD"/>
         </patternFill>
       </fill>
     </dxf>
@@ -114,16 +116,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFB4C7E7"/>
-          <bgColor rgb="FFB4C7E7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF8CBAD"/>
-          <bgColor rgb="FFF8CBAD"/>
+          <fgColor rgb="FFD9D2E9"/>
+          <bgColor rgb="FFD9D2E9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -138,16 +132,24 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFD9D2E9"/>
-          <bgColor rgb="FFD9D2E9"/>
+          <fgColor rgb="FFC5E0B4"/>
+          <bgColor rgb="FFC5E0B4"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFC5E0B4"/>
-          <bgColor rgb="FFC5E0B4"/>
+          <fgColor rgb="FFB4C7E7"/>
+          <bgColor rgb="FFB4C7E7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE699"/>
+          <bgColor rgb="FFFFE699"/>
         </patternFill>
       </fill>
     </dxf>
@@ -218,16 +220,16 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFFE699"/>
-          <bgColor rgb="FFFFE699"/>
+          <fgColor rgb="FFB4C7E7"/>
+          <bgColor rgb="FFB4C7E7"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFB4C7E7"/>
-          <bgColor rgb="FFB4C7E7"/>
+          <fgColor rgb="FFFFE699"/>
+          <bgColor rgb="FFFFE699"/>
         </patternFill>
       </fill>
     </dxf>
@@ -589,15 +591,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:BD38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="AZ8" sqref="AZ8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -617,9 +619,9 @@
     <col width="13" customWidth="1" min="13" max="13"/>
     <col width="17" customWidth="1" min="14" max="14"/>
     <col width="23" customWidth="1" min="15" max="15"/>
-    <col width="15" customWidth="1" min="16" max="16"/>
-    <col width="17" customWidth="1" min="17" max="17"/>
-    <col width="31" customWidth="1" min="18" max="18"/>
+    <col hidden="1" width="15" customWidth="1" min="16" max="16"/>
+    <col hidden="1" width="17" customWidth="1" min="17" max="17"/>
+    <col hidden="1" width="31" customWidth="1" min="18" max="18"/>
     <col width="25" customWidth="1" min="19" max="19"/>
     <col width="36" customWidth="1" min="20" max="20"/>
     <col width="50" customWidth="1" min="21" max="21"/>
@@ -1111,7 +1113,7 @@
         </is>
       </c>
     </row>
-    <row r="3">
+    <row r="3" hidden="1">
       <c r="A3" t="inlineStr">
         <is>
           <t>Pre-MQL ready for validation: Riccardo Infanti from RaceUp Team</t>
@@ -1237,7 +1239,7 @@
           <t>Not Matched</t>
         </is>
       </c>
-      <c r="AM3" t="inlineStr">
+      <c r="AM3" s="2" t="inlineStr">
         <is>
           <t>https://infineoncommunity.com/marketing-qualification?id=1490890DC2AFCF91A01A-10&amp;accType=&amp;loc=EMEA</t>
         </is>
@@ -1262,6 +1264,11 @@
           <t>Valid Company Domain</t>
         </is>
       </c>
+      <c r="AZ3" t="inlineStr">
+        <is>
+          <t>Rejected Marketing</t>
+        </is>
+      </c>
       <c r="BA3" t="inlineStr">
         <is>
           <t>Not Started</t>
@@ -1274,7 +1281,7 @@
       </c>
       <c r="BD3" t="inlineStr">
         <is>
-          <t>Not processed - No folder selected</t>
+          <t>Failed - Email not found in source folder</t>
         </is>
       </c>
     </row>
@@ -1435,7 +1442,7 @@
         </is>
       </c>
     </row>
-    <row r="5">
+    <row r="5" hidden="1">
       <c r="A5" t="inlineStr">
         <is>
           <t>Pre-MQL ready for validation: Stephen Pringle from MaxxCAM</t>
@@ -1466,7 +1473,7 @@
           <t>Pringle</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="G5" s="2" t="inlineStr">
         <is>
           <t>stephen@maxxcam.com</t>
         </is>
@@ -1561,7 +1568,7 @@
           <t>Not Matched</t>
         </is>
       </c>
-      <c r="AM5" t="inlineStr">
+      <c r="AM5" s="2" t="inlineStr">
         <is>
           <t>https://infineoncommunity.com/marketing-qualification?id=1490558B110D9939CAD7-3&amp;accType=&amp;loc=EMEA</t>
         </is>
@@ -1586,6 +1593,11 @@
           <t>Valid Company Domain</t>
         </is>
       </c>
+      <c r="AZ5" t="inlineStr">
+        <is>
+          <t>EBV/Avnet</t>
+        </is>
+      </c>
       <c r="BA5" t="inlineStr">
         <is>
           <t>Not Started</t>
@@ -1598,11 +1610,11 @@
       </c>
       <c r="BD5" t="inlineStr">
         <is>
-          <t>Not processed - No folder selected</t>
+          <t>Failed - Email not found in source folder</t>
         </is>
       </c>
     </row>
-    <row r="6">
+    <row r="6" hidden="1">
       <c r="A6" t="inlineStr">
         <is>
           <t>Pre-MQL ready for validation: Murat Aktürk from Qest GmbH</t>
@@ -1633,7 +1645,7 @@
           <t>Aktürk</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="G6" s="2" t="inlineStr">
         <is>
           <t>murat.aktuerk@qest.de</t>
         </is>
@@ -1728,7 +1740,7 @@
           <t>Not Matched</t>
         </is>
       </c>
-      <c r="AM6" t="inlineStr">
+      <c r="AM6" s="2" t="inlineStr">
         <is>
           <t>https://infineoncommunity.com/marketing-qualification?id=2123965567E7642611D5-1&amp;accType=&amp;loc=EMEA</t>
         </is>
@@ -1753,6 +1765,11 @@
           <t>Valid Company Domain</t>
         </is>
       </c>
+      <c r="AZ6" t="inlineStr">
+        <is>
+          <t>EBV/Avnet</t>
+        </is>
+      </c>
       <c r="BA6" t="inlineStr">
         <is>
           <t>Not Started</t>
@@ -1765,7 +1782,7 @@
       </c>
       <c r="BD6" t="inlineStr">
         <is>
-          <t>Not processed - No folder selected</t>
+          <t>Failed - Email not found in source folder</t>
         </is>
       </c>
     </row>
@@ -2062,7 +2079,7 @@
           <t>Not Matched</t>
         </is>
       </c>
-      <c r="AM8" t="inlineStr">
+      <c r="AM8" s="2" t="inlineStr">
         <is>
           <t>https://infineoncommunity.com/marketing-qualification?id=2039846037FC6C6D092E-2&amp;accType=&amp;loc=EMEA</t>
         </is>
@@ -2087,6 +2104,11 @@
           <t>Free Mailer</t>
         </is>
       </c>
+      <c r="AZ8" t="inlineStr">
+        <is>
+          <t>Rejected Marketing</t>
+        </is>
+      </c>
       <c r="BA8" t="inlineStr">
         <is>
           <t>Not Started</t>
@@ -2099,7 +2121,7 @@
       </c>
       <c r="BD8" t="inlineStr">
         <is>
-          <t>Not processed - No folder selected</t>
+          <t>✓ Moved to Rejected Marketing</t>
         </is>
       </c>
     </row>
@@ -2437,7 +2459,7 @@
         </is>
       </c>
     </row>
-    <row r="11">
+    <row r="11" hidden="1">
       <c r="A11" t="inlineStr">
         <is>
           <t>Pre-MQL ready for validation: Mat Wu from Pulse</t>
@@ -2468,7 +2490,7 @@
           <t>Wu</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="G11" s="2" t="inlineStr">
         <is>
           <t>matthias.wukovits@pulsvario.com</t>
         </is>
@@ -2573,7 +2595,7 @@
           <t>Not Matched</t>
         </is>
       </c>
-      <c r="AM11" t="inlineStr">
+      <c r="AM11" s="2" t="inlineStr">
         <is>
           <t>https://infineoncommunity.com/marketing-qualification?id=1037438484B6C592D97F-6&amp;accType=&amp;loc=EMEA</t>
         </is>
@@ -2598,6 +2620,11 @@
           <t>Domain Mismatch</t>
         </is>
       </c>
+      <c r="AZ11" t="inlineStr">
+        <is>
+          <t>EBV/Avnet</t>
+        </is>
+      </c>
       <c r="BA11" t="inlineStr">
         <is>
           <t>Not Started</t>
@@ -2610,11 +2637,11 @@
       </c>
       <c r="BD11" t="inlineStr">
         <is>
-          <t>Not processed - No folder selected</t>
+          <t>Failed - Email not found in source folder</t>
         </is>
       </c>
     </row>
-    <row r="12">
+    <row r="12" hidden="1">
       <c r="A12" t="inlineStr">
         <is>
           <t>Pre-MQL ready for validation: Yasmine Baazizi from INSA rennes</t>
@@ -2645,7 +2672,7 @@
           <t>Baazizi</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="G12" s="2" t="inlineStr">
         <is>
           <t>yasmine.baazizi@insa-rennes.fr</t>
         </is>
@@ -2745,7 +2772,7 @@
           <t>Not Matched</t>
         </is>
       </c>
-      <c r="AM12" t="inlineStr">
+      <c r="AM12" s="2" t="inlineStr">
         <is>
           <t>https://infineoncommunity.com/marketing-qualification?id=212137685BC4F658FA9E-1&amp;accType=&amp;loc=EMEA</t>
         </is>
@@ -2770,6 +2797,11 @@
           <t>Valid Company Domain</t>
         </is>
       </c>
+      <c r="AZ12" t="inlineStr">
+        <is>
+          <t>Rejected Marketing</t>
+        </is>
+      </c>
       <c r="BA12" t="inlineStr">
         <is>
           <t>Not Started</t>
@@ -2782,7 +2814,7 @@
       </c>
       <c r="BD12" t="inlineStr">
         <is>
-          <t>Not processed - No folder selected</t>
+          <t>Failed - Email not found in source folder</t>
         </is>
       </c>
     </row>
@@ -3272,7 +3304,7 @@
         </is>
       </c>
     </row>
-    <row r="16">
+    <row r="16" hidden="1">
       <c r="A16" t="inlineStr">
         <is>
           <t>Pre-MQL ready for validation: Jean-Marc Duges from HAM radio</t>
@@ -3303,7 +3335,7 @@
           <t>Duges</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="G16" s="2" t="inlineStr">
         <is>
           <t>jm@duges.fr</t>
         </is>
@@ -3403,7 +3435,7 @@
           <t>Not Matched</t>
         </is>
       </c>
-      <c r="AM16" t="inlineStr">
+      <c r="AM16" s="2" t="inlineStr">
         <is>
           <t>https://infineoncommunity.com/marketing-qualification?id=21224478CB6F8AB3BB6A-1&amp;accType=&amp;loc=EMEA</t>
         </is>
@@ -3428,6 +3460,11 @@
           <t>Domain Mismatch</t>
         </is>
       </c>
+      <c r="AZ16" t="inlineStr">
+        <is>
+          <t>Rejected Marketing</t>
+        </is>
+      </c>
       <c r="BA16" t="inlineStr">
         <is>
           <t>Not Started</t>
@@ -3440,7 +3477,7 @@
       </c>
       <c r="BD16" t="inlineStr">
         <is>
-          <t>Not processed - No folder selected</t>
+          <t>Failed - Email not found in source folder</t>
         </is>
       </c>
     </row>
@@ -3930,7 +3967,7 @@
         </is>
       </c>
     </row>
-    <row r="20">
+    <row r="20" hidden="1">
       <c r="A20" t="inlineStr">
         <is>
           <t>Pre-MQL ready for validation: Fernando Oliveira from Lincad Ltd.</t>
@@ -3961,7 +3998,7 @@
           <t>Oliveira</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
+      <c r="G20" s="2" t="inlineStr">
         <is>
           <t>fernando.oliveira@lincad.co.uk</t>
         </is>
@@ -4061,7 +4098,7 @@
           <t>Not Matched</t>
         </is>
       </c>
-      <c r="AM20" t="inlineStr">
+      <c r="AM20" s="2" t="inlineStr">
         <is>
           <t>https://infineoncommunity.com/marketing-qualification?id=21239039F418630D9062-1&amp;accType=&amp;loc=EMEA</t>
         </is>
@@ -4086,6 +4123,11 @@
           <t>Valid Company Domain</t>
         </is>
       </c>
+      <c r="AZ20" t="inlineStr">
+        <is>
+          <t>EBV/Avnet</t>
+        </is>
+      </c>
       <c r="BA20" t="inlineStr">
         <is>
           <t>Not Started</t>
@@ -4098,11 +4140,11 @@
       </c>
       <c r="BD20" t="inlineStr">
         <is>
-          <t>Not processed - No folder selected</t>
+          <t>Failed - Email not found in source folder</t>
         </is>
       </c>
     </row>
-    <row r="21">
+    <row r="21" hidden="1">
       <c r="A21" t="inlineStr">
         <is>
           <t>Pre-MQL ready for validation: Hussein Ahmed from Zagzoog company</t>
@@ -4133,7 +4175,7 @@
           <t>Ahmed</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
+      <c r="G21" s="2" t="inlineStr">
         <is>
           <t>hlami@zagzoog.com</t>
         </is>
@@ -4228,7 +4270,7 @@
           <t>Not Matched</t>
         </is>
       </c>
-      <c r="AM21" t="inlineStr">
+      <c r="AM21" s="2" t="inlineStr">
         <is>
           <t>https://infineoncommunity.com/marketing-qualification?id=1465582C32304026DB43-5&amp;accType=&amp;loc=EMEA</t>
         </is>
@@ -4253,6 +4295,11 @@
           <t>Valid Company Domain</t>
         </is>
       </c>
+      <c r="AZ21" t="inlineStr">
+        <is>
+          <t>Rejected Marketing</t>
+        </is>
+      </c>
       <c r="BA21" t="inlineStr">
         <is>
           <t>Not Started</t>
@@ -4265,7 +4312,7 @@
       </c>
       <c r="BD21" t="inlineStr">
         <is>
-          <t>Not processed - No folder selected</t>
+          <t>Failed - Email not found in source folder</t>
         </is>
       </c>
     </row>
@@ -4431,7 +4478,7 @@
         </is>
       </c>
     </row>
-    <row r="23">
+    <row r="23" hidden="1">
       <c r="A23" t="inlineStr">
         <is>
           <t>Pre-MQL ready for validation: Lars Olsson from Swede electronics AB</t>
@@ -4462,7 +4509,7 @@
           <t>Olsson</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr">
+      <c r="G23" s="2" t="inlineStr">
         <is>
           <t>lars.olsson@swedeelec.se</t>
         </is>
@@ -4552,7 +4599,7 @@
           <t>Not Matched</t>
         </is>
       </c>
-      <c r="AM23" t="inlineStr">
+      <c r="AM23" s="2" t="inlineStr">
         <is>
           <t>https://infineoncommunity.com/marketing-qualification?id=1510714EEC5393150492-2&amp;accType=&amp;loc=EMEA</t>
         </is>
@@ -4577,6 +4624,11 @@
           <t>Valid Company Domain</t>
         </is>
       </c>
+      <c r="AZ23" t="inlineStr">
+        <is>
+          <t>EBV/Avnet</t>
+        </is>
+      </c>
       <c r="BA23" t="inlineStr">
         <is>
           <t>Not Started</t>
@@ -4589,7 +4641,7 @@
       </c>
       <c r="BD23" t="inlineStr">
         <is>
-          <t>Not processed - No folder selected</t>
+          <t>Failed - Email not found in source folder</t>
         </is>
       </c>
     </row>
@@ -4927,7 +4979,7 @@
         </is>
       </c>
     </row>
-    <row r="26">
+    <row r="26" hidden="1">
       <c r="A26" t="inlineStr">
         <is>
           <t>Pre-MQL ready for validation: Horst Mäder from enerkite GmbH</t>
@@ -4958,7 +5010,7 @@
           <t>Mäder</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr">
+      <c r="G26" s="2" t="inlineStr">
         <is>
           <t>h.maeder@enerkite.de</t>
         </is>
@@ -5053,7 +5105,7 @@
           <t>Not Matched</t>
         </is>
       </c>
-      <c r="AM26" t="inlineStr">
+      <c r="AM26" s="2" t="inlineStr">
         <is>
           <t>https://infineoncommunity.com/marketing-qualification?id=21220032E485847709C5-1&amp;accType=&amp;loc=EMEA</t>
         </is>
@@ -5078,6 +5130,11 @@
           <t>Valid Company Domain</t>
         </is>
       </c>
+      <c r="AZ26" t="inlineStr">
+        <is>
+          <t>EBV/Avnet</t>
+        </is>
+      </c>
       <c r="BA26" t="inlineStr">
         <is>
           <t>Not Started</t>
@@ -5090,7 +5147,7 @@
       </c>
       <c r="BD26" t="inlineStr">
         <is>
-          <t>Not processed - No folder selected</t>
+          <t>Failed - Email not found in source folder</t>
         </is>
       </c>
     </row>
@@ -5266,7 +5323,7 @@
         </is>
       </c>
     </row>
-    <row r="28">
+    <row r="28" hidden="1">
       <c r="A28" t="inlineStr">
         <is>
           <t>Pre-MQL ready for validation: Marc van Heijningen from TNO</t>
@@ -5297,7 +5354,7 @@
           <t>van Heijningen</t>
         </is>
       </c>
-      <c r="G28" t="inlineStr">
+      <c r="G28" s="2" t="inlineStr">
         <is>
           <t>marc.vanheijningen@tno.nl</t>
         </is>
@@ -5397,7 +5454,7 @@
           <t>Not Matched</t>
         </is>
       </c>
-      <c r="AM28" t="inlineStr">
+      <c r="AM28" s="2" t="inlineStr">
         <is>
           <t>https://infineoncommunity.com/marketing-qualification?id=2110872E7FB077A9CA6B-1&amp;accType=&amp;loc=EMEA</t>
         </is>
@@ -5422,6 +5479,11 @@
           <t>Valid Company Domain</t>
         </is>
       </c>
+      <c r="AZ28" t="inlineStr">
+        <is>
+          <t>EBV/Avnet</t>
+        </is>
+      </c>
       <c r="BA28" t="inlineStr">
         <is>
           <t>Not Started</t>
@@ -5434,11 +5496,11 @@
       </c>
       <c r="BD28" t="inlineStr">
         <is>
-          <t>Not processed - No folder selected</t>
+          <t>Failed - Email not found in source folder</t>
         </is>
       </c>
     </row>
-    <row r="29">
+    <row r="29" hidden="1">
       <c r="A29" t="inlineStr">
         <is>
           <t>Pre-MQL ready for validation: Joachim Schneider from Driventic GmbH</t>
@@ -5469,7 +5531,7 @@
           <t>Schneider</t>
         </is>
       </c>
-      <c r="G29" t="inlineStr">
+      <c r="G29" s="2" t="inlineStr">
         <is>
           <t>Joachim.Schneider@driventic.com</t>
         </is>
@@ -5574,7 +5636,7 @@
           <t>Not Matched</t>
         </is>
       </c>
-      <c r="AM29" t="inlineStr">
+      <c r="AM29" s="2" t="inlineStr">
         <is>
           <t>https://infineoncommunity.com/marketing-qualification?id=20995432086073B486ED-1&amp;accType=&amp;loc=EMEA</t>
         </is>
@@ -5599,6 +5661,11 @@
           <t>Valid Company Domain</t>
         </is>
       </c>
+      <c r="AZ29" t="inlineStr">
+        <is>
+          <t>EBV/Avnet</t>
+        </is>
+      </c>
       <c r="BA29" t="inlineStr">
         <is>
           <t>Not Started</t>
@@ -5611,11 +5678,11 @@
       </c>
       <c r="BD29" t="inlineStr">
         <is>
-          <t>Not processed - No folder selected</t>
+          <t>Failed - Email not found in source folder</t>
         </is>
       </c>
     </row>
-    <row r="30">
+    <row r="30" hidden="1">
       <c r="A30" t="inlineStr">
         <is>
           <t>Pre-MQL ready for validation: BERTIN Thibault from CEA Grenoble</t>
@@ -5646,7 +5713,7 @@
           <t>Thibault</t>
         </is>
       </c>
-      <c r="G30" t="inlineStr">
+      <c r="G30" s="2" t="inlineStr">
         <is>
           <t>thibault.bertinrivieredelasouchere@cea.fr</t>
         </is>
@@ -5746,7 +5813,7 @@
           <t>Not Matched</t>
         </is>
       </c>
-      <c r="AM30" t="inlineStr">
+      <c r="AM30" s="2" t="inlineStr">
         <is>
           <t>https://infineoncommunity.com/marketing-qualification?id=20398872CABE7F39C175-2&amp;accType=&amp;loc=EMEA</t>
         </is>
@@ -5771,6 +5838,11 @@
           <t>Valid Company Domain</t>
         </is>
       </c>
+      <c r="AZ30" t="inlineStr">
+        <is>
+          <t>EBV/Avnet</t>
+        </is>
+      </c>
       <c r="BA30" t="inlineStr">
         <is>
           <t>Not Started</t>
@@ -5783,7 +5855,7 @@
       </c>
       <c r="BD30" t="inlineStr">
         <is>
-          <t>Not processed - No folder selected</t>
+          <t>Failed - Email not found in source folder</t>
         </is>
       </c>
     </row>
@@ -6147,7 +6219,7 @@
         </is>
       </c>
     </row>
-    <row r="33">
+    <row r="33" hidden="1">
       <c r="A33" t="inlineStr">
         <is>
           <t>Pre-MQL ready for validation: Laszlo Kovacs from Sympat engineering Kft.</t>
@@ -6178,7 +6250,7 @@
           <t>Kovacs</t>
         </is>
       </c>
-      <c r="G33" t="inlineStr">
+      <c r="G33" s="2" t="inlineStr">
         <is>
           <t>laszlo.kovacs@sympat.hu</t>
         </is>
@@ -6273,7 +6345,7 @@
           <t>Not Matched</t>
         </is>
       </c>
-      <c r="AM33" t="inlineStr">
+      <c r="AM33" s="2" t="inlineStr">
         <is>
           <t>https://infineoncommunity.com/marketing-qualification?id=1851758853BFC512F9F5-4&amp;accType=&amp;loc=EMEA</t>
         </is>
@@ -6299,6 +6371,11 @@
           <t>Valid Company Domain</t>
         </is>
       </c>
+      <c r="AZ33" t="inlineStr">
+        <is>
+          <t>Rejected Marketing</t>
+        </is>
+      </c>
       <c r="BA33" t="inlineStr">
         <is>
           <t>Not Started</t>
@@ -6311,11 +6388,11 @@
       </c>
       <c r="BD33" t="inlineStr">
         <is>
-          <t>Not processed - No folder selected</t>
+          <t>Failed - Email not found in source folder</t>
         </is>
       </c>
     </row>
-    <row r="34">
+    <row r="34" hidden="1">
       <c r="A34" t="inlineStr">
         <is>
           <t>Pre-MQL ready for validation: Pascal Engel from ENGEL-SysDev GmbH</t>
@@ -6346,7 +6423,7 @@
           <t>Engel</t>
         </is>
       </c>
-      <c r="G34" t="inlineStr">
+      <c r="G34" s="2" t="inlineStr">
         <is>
           <t>pe@engel-sysdev.de</t>
         </is>
@@ -6451,7 +6528,7 @@
           <t>Not Matched</t>
         </is>
       </c>
-      <c r="AM34" t="inlineStr">
+      <c r="AM34" s="2" t="inlineStr">
         <is>
           <t>https://infineoncommunity.com/marketing-qualification?id=1750993C19E0D5E90F96-2&amp;accType=&amp;loc=EMEA</t>
         </is>
@@ -6476,6 +6553,11 @@
           <t>Valid Company Domain</t>
         </is>
       </c>
+      <c r="AZ34" t="inlineStr">
+        <is>
+          <t>Rejected Marketing</t>
+        </is>
+      </c>
       <c r="BA34" t="inlineStr">
         <is>
           <t>Not Started</t>
@@ -6488,7 +6570,7 @@
       </c>
       <c r="BD34" t="inlineStr">
         <is>
-          <t>Not processed - No folder selected</t>
+          <t>Failed - Email not found in source folder</t>
         </is>
       </c>
     </row>
@@ -6659,7 +6741,7 @@
         </is>
       </c>
     </row>
-    <row r="36">
+    <row r="36" hidden="1">
       <c r="A36" t="inlineStr">
         <is>
           <t>Pre-MQL ready for validation: Mika Hämäläinen from Homeuse</t>
@@ -6690,7 +6772,7 @@
           <t>Hämäläinen</t>
         </is>
       </c>
-      <c r="G36" t="inlineStr">
+      <c r="G36" s="2" t="inlineStr">
         <is>
           <t>hamy@oh4kpn.org</t>
         </is>
@@ -6790,7 +6872,7 @@
           <t>Not Matched</t>
         </is>
       </c>
-      <c r="AM36" t="inlineStr">
+      <c r="AM36" s="2" t="inlineStr">
         <is>
           <t>https://infineoncommunity.com/marketing-qualification?id=21221722EC258C05D63A-1&amp;accType=&amp;loc=EMEA</t>
         </is>
@@ -6815,6 +6897,11 @@
           <t>Domain Mismatch</t>
         </is>
       </c>
+      <c r="AZ36" t="inlineStr">
+        <is>
+          <t>Rejected Marketing</t>
+        </is>
+      </c>
       <c r="BA36" t="inlineStr">
         <is>
           <t>Not Started</t>
@@ -6827,7 +6914,7 @@
       </c>
       <c r="BD36" t="inlineStr">
         <is>
-          <t>Not processed - No folder selected</t>
+          <t>Failed - Email not found in source folder</t>
         </is>
       </c>
     </row>
@@ -6988,7 +7075,7 @@
         </is>
       </c>
     </row>
-    <row r="38">
+    <row r="38" hidden="1">
       <c r="A38" t="inlineStr">
         <is>
           <t>Pre-MQL ready for validation: Roberto Lampugnani from AiM Tech s.r.l.</t>
@@ -7019,7 +7106,7 @@
           <t>Lampugnani</t>
         </is>
       </c>
-      <c r="G38" t="inlineStr">
+      <c r="G38" s="2" t="inlineStr">
         <is>
           <t>roberto.lampugnani@aim-sportline.com</t>
         </is>
@@ -7124,7 +7211,7 @@
           <t>Not Matched</t>
         </is>
       </c>
-      <c r="AM38" t="inlineStr">
+      <c r="AM38" s="2" t="inlineStr">
         <is>
           <t>https://infineoncommunity.com/marketing-qualification?id=2057332B1177F2CB4D77-1&amp;accType=&amp;loc=EMEA</t>
         </is>
@@ -7149,6 +7236,11 @@
           <t>Domain Mismatch</t>
         </is>
       </c>
+      <c r="AZ38" t="inlineStr">
+        <is>
+          <t>EBV/Avnet</t>
+        </is>
+      </c>
       <c r="BA38" t="inlineStr">
         <is>
           <t>Not Started</t>
@@ -7161,31 +7253,38 @@
       </c>
       <c r="BD38" t="inlineStr">
         <is>
-          <t>Not processed - No folder selected</t>
+          <t>Failed - Email not found in source folder</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:BD38">
+    <filterColumn colId="45" hiddenButton="0" showButton="1">
+      <filters>
+        <filter val="Free Mailer"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="A2:BC38">
-    <cfRule type="expression" priority="186" dxfId="4">
+    <cfRule type="expression" priority="149" dxfId="8">
+      <formula>$AZ2="Arrow"</formula>
+    </cfRule>
+    <cfRule type="expression" priority="186" dxfId="7">
       <formula>$AZ2="EBV/Avnet"</formula>
     </cfRule>
-    <cfRule type="expression" priority="149" dxfId="2">
-      <formula>$AZ2="Arrow"</formula>
-    </cfRule>
-    <cfRule type="expression" priority="223" dxfId="8">
+    <cfRule type="expression" priority="223" dxfId="6">
       <formula>$AZ2="Future"</formula>
     </cfRule>
-    <cfRule type="expression" priority="260" dxfId="6">
+    <cfRule type="expression" priority="260" dxfId="5">
       <formula>$AZ2="Non-EBV Leads"</formula>
     </cfRule>
-    <cfRule type="expression" priority="297" dxfId="7">
+    <cfRule type="expression" priority="297" dxfId="4">
       <formula>$AZ2="Other Distribution Partners"</formula>
     </cfRule>
     <cfRule type="expression" priority="334" dxfId="3">
       <formula>$AZ2="Rutronik"</formula>
     </cfRule>
-    <cfRule type="expression" priority="371" dxfId="5">
+    <cfRule type="expression" priority="371" dxfId="2">
       <formula>$AZ2="Rejected Marketing"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7218,6 +7317,42 @@
       <formula1>"Arrow,EBV/Avnet,Future,Non-EBV Leads,Other Distribution Partners,Rutronik,Rejected Marketing"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="AM3" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G5" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="AM5" r:id="rId3"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G6" r:id="rId4"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="AM6" r:id="rId5"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="AM8" r:id="rId6"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G11" r:id="rId7"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="AM11" r:id="rId8"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G12" r:id="rId9"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="AM12" r:id="rId10"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G16" r:id="rId11"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="AM16" r:id="rId12"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G20" r:id="rId13"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="AM20" r:id="rId14"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G21" r:id="rId15"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="AM21" r:id="rId16"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G23" r:id="rId17"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="AM23" r:id="rId18"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G26" r:id="rId19"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="AM26" r:id="rId20"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G28" r:id="rId21"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="AM28" r:id="rId22"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G29" r:id="rId23"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="AM29" r:id="rId24"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G30" r:id="rId25"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="AM30" r:id="rId26"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G33" r:id="rId27"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="AM33" r:id="rId28"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G34" r:id="rId29"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="AM34" r:id="rId30"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G36" r:id="rId31"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="AM36" r:id="rId32"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G38" r:id="rId33"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="AM38" r:id="rId34"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -7230,9 +7365,9 @@
   </sheetPr>
   <dimension ref="A1:BC5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AY17" sqref="AY17"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -8300,26 +8435,26 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:BB5">
-    <cfRule type="expression" priority="21" dxfId="8">
+    <cfRule type="expression" priority="13" dxfId="8">
+      <formula>$AY2="Arrow"</formula>
+    </cfRule>
+    <cfRule type="expression" priority="17" dxfId="7">
+      <formula>$AY2="EBV/Avnet"</formula>
+    </cfRule>
+    <cfRule type="expression" priority="21" dxfId="6">
       <formula>$AY2="Future"</formula>
     </cfRule>
-    <cfRule type="expression" priority="29" dxfId="7">
-      <formula>$AY2="Other Distribution Partners"</formula>
-    </cfRule>
-    <cfRule type="expression" priority="25" dxfId="6">
+    <cfRule type="expression" priority="25" dxfId="5">
       <formula>$AY2="Non-EBV Leads"</formula>
     </cfRule>
-    <cfRule type="expression" priority="37" dxfId="5">
-      <formula>$AY2="Rejected Marketing"</formula>
-    </cfRule>
-    <cfRule type="expression" priority="17" dxfId="4">
-      <formula>$AY2="EBV/Avnet"</formula>
+    <cfRule type="expression" priority="29" dxfId="4">
+      <formula>$AY2="Other Distribution Partners"</formula>
     </cfRule>
     <cfRule type="expression" priority="33" dxfId="3">
       <formula>$AY2="Rutronik"</formula>
     </cfRule>
-    <cfRule type="expression" priority="13" dxfId="2">
-      <formula>$AY2="Arrow"</formula>
+    <cfRule type="expression" priority="37" dxfId="2">
+      <formula>$AY2="Rejected Marketing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV2:AV5">

</xml_diff>